<commit_message>
Admin: building the send mail controller and the button to send a new password
</commit_message>
<xml_diff>
--- a/public/excel_files/Programas.xlsx
+++ b/public/excel_files/Programas.xlsx
@@ -11,24 +11,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="16">
   <si>
     <t>PWDAM</t>
   </si>
   <si>
-    <t>ING</t>
+    <t>IRC</t>
   </si>
   <si>
     <t>F369</t>
   </si>
   <si>
-    <t>SGBD</t>
+    <t>IT</t>
   </si>
   <si>
     <t>IPI</t>
   </si>
   <si>
+    <t>SGBD</t>
+  </si>
+  <si>
     <t>FM</t>
+  </si>
+  <si>
+    <t>ING</t>
   </si>
   <si>
     <t>CIC</t>
@@ -59,7 +65,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -68,6 +74,7 @@
     <font>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -97,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -105,9 +112,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -122,46 +129,49 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -413,7 +423,7 @@
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="4">
@@ -437,13 +447,13 @@
       <c r="I2" s="7"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="11">
         <v>1.59126321E8</v>
       </c>
       <c r="D3" s="4">
@@ -455,7 +465,7 @@
       <c r="F3" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H3" s="6">
@@ -464,11 +474,11 @@
       <c r="I3" s="7"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4">
         <v>1.23456871E8</v>
@@ -482,7 +492,7 @@
       <c r="F4" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H4" s="6">
@@ -491,11 +501,11 @@
       <c r="I4" s="7"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="4">
         <v>2.35689741E8</v>
@@ -509,7 +519,7 @@
       <c r="F5" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H5" s="6">
@@ -518,11 +528,11 @@
       <c r="I5" s="7"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>1</v>
+      <c r="A6" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="C6" s="4">
         <v>1.02543687E8</v>
@@ -536,7 +546,7 @@
       <c r="F6" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H6" s="6">
@@ -545,11 +555,11 @@
       <c r="I6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
+      <c r="A7" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="C7" s="4">
         <v>1.23456789E8</v>
@@ -563,7 +573,7 @@
       <c r="F7" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H7" s="6">
@@ -572,13 +582,13 @@
       <c r="I7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="11">
         <v>1.59126321E8</v>
       </c>
       <c r="D8" s="4">
@@ -590,7 +600,7 @@
       <c r="F8" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H8" s="6">
@@ -599,11 +609,11 @@
       <c r="I8" s="7"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" s="4">
         <v>2.35689741E8</v>
@@ -617,7 +627,7 @@
       <c r="F9" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H9" s="6">
@@ -626,11 +636,11 @@
       <c r="I9" s="7"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>1</v>
+      <c r="A10" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="C10" s="4">
         <v>1.02543687E8</v>
@@ -644,7 +654,7 @@
       <c r="F10" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H10" s="6">
@@ -653,11 +663,11 @@
       <c r="I10" s="7"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>6</v>
+      <c r="A11" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="C11" s="4">
         <v>1.23456789E8</v>
@@ -671,7 +681,7 @@
       <c r="F11" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H11" s="6">
@@ -680,13 +690,13 @@
       <c r="I11" s="7"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="11">
         <v>1.59126321E8</v>
       </c>
       <c r="D12" s="4">
@@ -698,7 +708,7 @@
       <c r="F12" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H12" s="6">
@@ -707,11 +717,11 @@
       <c r="I12" s="7"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C13" s="4">
         <v>1.23456871E8</v>
@@ -725,7 +735,7 @@
       <c r="F13" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H13" s="6">
@@ -734,11 +744,11 @@
       <c r="I13" s="7"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" s="4">
         <v>2.35689741E8</v>
@@ -752,7 +762,7 @@
       <c r="F14" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H14" s="6">
@@ -761,16 +771,16 @@
       <c r="I14" s="7"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>1</v>
+      <c r="A15" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="C15" s="4">
         <v>1.02543687E8</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="11">
         <v>2.0200121E7</v>
       </c>
       <c r="E15" s="4">
@@ -779,7 +789,7 @@
       <c r="F15" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H15" s="6">
@@ -788,16 +798,16 @@
       <c r="I15" s="7"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>6</v>
+      <c r="A16" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="C16" s="4">
         <v>1.23456789E8</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="11">
         <v>2.0200122E7</v>
       </c>
       <c r="E16" s="4">
@@ -806,7 +816,7 @@
       <c r="F16" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H16" s="6">
@@ -815,13 +825,13 @@
       <c r="I16" s="7"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="A17" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="11">
         <v>1.59126321E8</v>
       </c>
       <c r="D17" s="4">
@@ -833,7 +843,7 @@
       <c r="F17" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H17" s="6">
@@ -842,11 +852,11 @@
       <c r="I17" s="7"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C18" s="4">
         <v>1.23456871E8</v>
@@ -860,7 +870,7 @@
       <c r="F18" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H18" s="6">
@@ -869,11 +879,11 @@
       <c r="I18" s="7"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C19" s="4">
         <v>2.35689741E8</v>
@@ -887,7 +897,7 @@
       <c r="F19" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H19" s="6">
@@ -896,11 +906,11 @@
       <c r="I19" s="7"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>1</v>
+      <c r="A20" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="C20" s="4">
         <v>1.02543687E8</v>
@@ -914,7 +924,7 @@
       <c r="F20" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H20" s="6">
@@ -923,11 +933,11 @@
       <c r="I20" s="7"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>6</v>
+      <c r="A21" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="C21" s="4">
         <v>1.23456789E8</v>
@@ -941,7 +951,7 @@
       <c r="F21" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G21" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H21" s="6">
@@ -950,13 +960,13 @@
       <c r="I21" s="7"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="2" t="s">
+      <c r="A22" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="11">
         <v>1.59126321E8</v>
       </c>
       <c r="D22" s="4">
@@ -968,7 +978,7 @@
       <c r="F22" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="G22" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H22" s="6">
@@ -977,11 +987,11 @@
       <c r="I22" s="7"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C23" s="4">
         <v>1.23456871E8</v>
@@ -995,7 +1005,7 @@
       <c r="F23" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G23" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H23" s="6">
@@ -1004,11 +1014,11 @@
       <c r="I23" s="7"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C24" s="4">
         <v>2.35689741E8</v>
@@ -1022,7 +1032,7 @@
       <c r="F24" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G24" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H24" s="6">
@@ -1031,16 +1041,16 @@
       <c r="I24" s="7"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>1</v>
+      <c r="A25" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="C25" s="4">
         <v>1.02543687E8</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="11">
         <v>2.0200204E7</v>
       </c>
       <c r="E25" s="4">
@@ -1049,7 +1059,7 @@
       <c r="F25" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="G25" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H25" s="6">
@@ -1058,16 +1068,16 @@
       <c r="I25" s="7"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>6</v>
+      <c r="A26" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="C26" s="4">
         <v>1.23456789E8</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="11">
         <v>2.0200205E7</v>
       </c>
       <c r="E26" s="4">
@@ -1076,7 +1086,7 @@
       <c r="F26" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="G26" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H26" s="6">
@@ -1085,13 +1095,13 @@
       <c r="I26" s="7"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="2" t="s">
+      <c r="A27" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="11">
         <v>1.59126321E8</v>
       </c>
       <c r="D27" s="4">
@@ -1103,7 +1113,7 @@
       <c r="F27" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G27" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H27" s="6">
@@ -1112,11 +1122,11 @@
       <c r="I27" s="7"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C28" s="4">
         <v>1.23456871E8</v>
@@ -1130,7 +1140,7 @@
       <c r="F28" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="G28" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H28" s="6">
@@ -1139,11 +1149,11 @@
       <c r="I28" s="7"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C29" s="4">
         <v>2.35689741E8</v>
@@ -1157,7 +1167,7 @@
       <c r="F29" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="G29" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H29" s="6">
@@ -1166,11 +1176,11 @@
       <c r="I29" s="7"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>1</v>
+      <c r="A30" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="C30" s="4">
         <v>1.02543687E8</v>
@@ -1184,7 +1194,7 @@
       <c r="F30" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G30" s="11" t="s">
+      <c r="G30" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H30" s="6">
@@ -1193,11 +1203,11 @@
       <c r="I30" s="7"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>6</v>
+      <c r="A31" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="C31" s="4">
         <v>1.23456789E8</v>
@@ -1211,7 +1221,7 @@
       <c r="F31" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="G31" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H31" s="6">
@@ -1220,13 +1230,13 @@
       <c r="I31" s="7"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="2" t="s">
+      <c r="A32" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="11">
         <v>1.59126321E8</v>
       </c>
       <c r="D32" s="4">
@@ -1238,7 +1248,7 @@
       <c r="F32" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="G32" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H32" s="6">
@@ -1247,11 +1257,11 @@
       <c r="I32" s="7"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C33" s="4">
         <v>1.23456871E8</v>
@@ -1265,7 +1275,7 @@
       <c r="F33" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G33" s="11" t="s">
+      <c r="G33" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H33" s="6">
@@ -1274,11 +1284,11 @@
       <c r="I33" s="7"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C34" s="4">
         <v>2.35689741E8</v>
@@ -1292,7 +1302,7 @@
       <c r="F34" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G34" s="11" t="s">
+      <c r="G34" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H34" s="6">
@@ -1301,11 +1311,11 @@
       <c r="I34" s="7"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>1</v>
+      <c r="A35" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="C35" s="4">
         <v>1.02543687E8</v>
@@ -1319,7 +1329,7 @@
       <c r="F35" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="G35" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H35" s="6">
@@ -1328,11 +1338,11 @@
       <c r="I35" s="7"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>6</v>
+      <c r="A36" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="C36" s="4">
         <v>1.23456789E8</v>
@@ -1346,7 +1356,7 @@
       <c r="F36" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G36" s="11" t="s">
+      <c r="G36" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H36" s="6">
@@ -1355,13 +1365,13 @@
       <c r="I36" s="7"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" s="2" t="s">
+      <c r="A37" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C37" s="11">
         <v>1.59126321E8</v>
       </c>
       <c r="D37" s="4">
@@ -1373,7 +1383,7 @@
       <c r="F37" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G37" s="11" t="s">
+      <c r="G37" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H37" s="6">
@@ -1382,11 +1392,11 @@
       <c r="I37" s="7"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C38" s="4">
         <v>1.23456871E8</v>
@@ -1400,7 +1410,7 @@
       <c r="F38" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G38" s="11" t="s">
+      <c r="G38" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H38" s="6">
@@ -1409,11 +1419,11 @@
       <c r="I38" s="7"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C39" s="4">
         <v>2.35689741E8</v>
@@ -1427,7 +1437,7 @@
       <c r="F39" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G39" s="11" t="s">
+      <c r="G39" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H39" s="6">
@@ -1436,11 +1446,11 @@
       <c r="I39" s="7"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>1</v>
+      <c r="A40" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="C40" s="4">
         <v>1.02543687E8</v>
@@ -1454,7 +1464,7 @@
       <c r="F40" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G40" s="11" t="s">
+      <c r="G40" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H40" s="6">
@@ -1463,11 +1473,11 @@
       <c r="I40" s="7"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>6</v>
+      <c r="A41" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="C41" s="4">
         <v>1.23456789E8</v>
@@ -1481,7 +1491,7 @@
       <c r="F41" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G41" s="11" t="s">
+      <c r="G41" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H41" s="6">
@@ -1490,13 +1500,13 @@
       <c r="I41" s="7"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" s="2" t="s">
+      <c r="A42" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="10">
+      <c r="C42" s="11">
         <v>1.59126321E8</v>
       </c>
       <c r="D42" s="4">
@@ -1508,7 +1518,7 @@
       <c r="F42" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G42" s="11" t="s">
+      <c r="G42" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H42" s="6">
@@ -1517,11 +1527,11 @@
       <c r="I42" s="7"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C43" s="4">
         <v>1.23456871E8</v>
@@ -1535,7 +1545,7 @@
       <c r="F43" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G43" s="11" t="s">
+      <c r="G43" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H43" s="6">
@@ -1544,16 +1554,16 @@
       <c r="I43" s="7"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C44" s="4">
         <v>2.35689741E8</v>
       </c>
-      <c r="D44" s="10">
+      <c r="D44" s="11">
         <v>2.0200302E7</v>
       </c>
       <c r="E44" s="4">
@@ -1562,7 +1572,7 @@
       <c r="F44" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G44" s="11" t="s">
+      <c r="G44" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H44" s="6">
@@ -1571,16 +1581,16 @@
       <c r="I44" s="7"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>1</v>
+      <c r="A45" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="C45" s="4">
         <v>1.02543687E8</v>
       </c>
-      <c r="D45" s="10">
+      <c r="D45" s="11">
         <v>2.0200303E7</v>
       </c>
       <c r="E45" s="4">
@@ -1589,7 +1599,7 @@
       <c r="F45" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G45" s="11" t="s">
+      <c r="G45" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H45" s="6">
@@ -1598,16 +1608,16 @@
       <c r="I45" s="7"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>6</v>
+      <c r="A46" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="C46" s="4">
         <v>1.23456789E8</v>
       </c>
-      <c r="D46" s="10">
+      <c r="D46" s="11">
         <v>2.0200304E7</v>
       </c>
       <c r="E46" s="4">
@@ -1616,7 +1626,7 @@
       <c r="F46" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G46" s="11" t="s">
+      <c r="G46" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H46" s="6">
@@ -1625,13 +1635,13 @@
       <c r="I46" s="7"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="2" t="s">
+      <c r="A47" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C47" s="10">
+      <c r="C47" s="11">
         <v>1.59126321E8</v>
       </c>
       <c r="D47" s="4">
@@ -1643,7 +1653,7 @@
       <c r="F47" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G47" s="11" t="s">
+      <c r="G47" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H47" s="6">
@@ -1652,11 +1662,11 @@
       <c r="I47" s="7"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C48" s="4">
         <v>1.23456871E8</v>
@@ -1670,7 +1680,7 @@
       <c r="F48" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G48" s="11" t="s">
+      <c r="G48" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H48" s="6">
@@ -1679,11 +1689,11 @@
       <c r="I48" s="7"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C49" s="4">
         <v>2.35689741E8</v>
@@ -1697,7 +1707,7 @@
       <c r="F49" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G49" s="11" t="s">
+      <c r="G49" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H49" s="6">
@@ -1706,11 +1716,11 @@
       <c r="I49" s="7"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>1</v>
+      <c r="A50" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="C50" s="4">
         <v>1.02543687E8</v>
@@ -1724,7 +1734,7 @@
       <c r="F50" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G50" s="11" t="s">
+      <c r="G50" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H50" s="6">
@@ -1733,11 +1743,11 @@
       <c r="I50" s="7"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>6</v>
+      <c r="A51" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="C51" s="4">
         <v>1.23456789E8</v>
@@ -1751,7 +1761,7 @@
       <c r="F51" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G51" s="11" t="s">
+      <c r="G51" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H51" s="6">
@@ -1760,13 +1770,13 @@
       <c r="I51" s="7"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="2" t="s">
+      <c r="A52" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C52" s="10">
+      <c r="C52" s="11">
         <v>1.59126321E8</v>
       </c>
       <c r="D52" s="4">
@@ -1778,7 +1788,7 @@
       <c r="F52" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G52" s="11" t="s">
+      <c r="G52" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H52" s="6">
@@ -1787,11 +1797,11 @@
       <c r="I52" s="7"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C53" s="3">
         <v>1.23456871E8</v>
@@ -1805,7 +1815,7 @@
       <c r="F53" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G53" s="11" t="s">
+      <c r="G53" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H53" s="6">
@@ -1814,13 +1824,13 @@
       <c r="I53" s="7"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" s="12">
+        <v>6</v>
+      </c>
+      <c r="C54" s="13">
         <v>2.35689741E8</v>
       </c>
       <c r="D54" s="4">
@@ -1832,7 +1842,7 @@
       <c r="F54" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G54" s="11" t="s">
+      <c r="G54" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H54" s="6">
@@ -1841,11 +1851,11 @@
       <c r="I54" s="7"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>1</v>
+      <c r="A55" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="C55" s="4">
         <v>1.02543687E8</v>
@@ -1859,7 +1869,7 @@
       <c r="F55" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G55" s="11" t="s">
+      <c r="G55" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H55" s="6">
@@ -1868,11 +1878,11 @@
       <c r="I55" s="7"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>6</v>
+      <c r="A56" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="C56" s="4">
         <v>1.23456789E8</v>
@@ -1886,7 +1896,7 @@
       <c r="F56" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G56" s="11" t="s">
+      <c r="G56" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H56" s="6">
@@ -1895,13 +1905,13 @@
       <c r="I56" s="7"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B57" s="2" t="s">
+      <c r="A57" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C57" s="10">
+      <c r="C57" s="11">
         <v>1.59126321E8</v>
       </c>
       <c r="D57" s="4">
@@ -1913,7 +1923,7 @@
       <c r="F57" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G57" s="11" t="s">
+      <c r="G57" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H57" s="6">
@@ -1922,11 +1932,11 @@
       <c r="I57" s="7"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C58" s="4">
         <v>1.23456871E8</v>
@@ -1940,7 +1950,7 @@
       <c r="F58" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G58" s="11" t="s">
+      <c r="G58" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H58" s="6">
@@ -1949,11 +1959,11 @@
       <c r="I58" s="7"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C59" s="4">
         <v>2.35689741E8</v>
@@ -1967,7 +1977,7 @@
       <c r="F59" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G59" s="11" t="s">
+      <c r="G59" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H59" s="6">
@@ -1976,11 +1986,11 @@
       <c r="I59" s="7"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>1</v>
+      <c r="A60" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="C60" s="4">
         <v>1.02543687E8</v>
@@ -1994,7 +2004,7 @@
       <c r="F60" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G60" s="11" t="s">
+      <c r="G60" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H60" s="6">
@@ -2003,11 +2013,11 @@
       <c r="I60" s="7"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>6</v>
+      <c r="A61" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="C61" s="4">
         <v>1.23456789E8</v>
@@ -2021,7 +2031,7 @@
       <c r="F61" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G61" s="11" t="s">
+      <c r="G61" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H61" s="6">
@@ -2030,13 +2040,13 @@
       <c r="I61" s="7"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B62" s="2" t="s">
+      <c r="A62" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B62" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C62" s="10">
+      <c r="C62" s="11">
         <v>1.59126321E8</v>
       </c>
       <c r="D62" s="4">
@@ -2048,7 +2058,7 @@
       <c r="F62" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G62" s="11" t="s">
+      <c r="G62" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H62" s="6">
@@ -2057,11 +2067,11 @@
       <c r="I62" s="7"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C63" s="4">
         <v>1.23456871E8</v>
@@ -2075,7 +2085,7 @@
       <c r="F63" s="4">
         <v>123000.0</v>
       </c>
-      <c r="G63" s="11" t="s">
+      <c r="G63" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H63" s="6">
@@ -2085,10 +2095,10 @@
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C64" s="4">
         <v>1.23456871E8</v>
@@ -2102,8 +2112,8 @@
       <c r="F64" s="3">
         <v>40000.0</v>
       </c>
-      <c r="G64" s="11" t="s">
-        <v>8</v>
+      <c r="G64" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="H64" s="6">
         <v>0.0</v>
@@ -2111,26 +2121,26 @@
       <c r="I64" s="7"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B65" s="2" t="s">
+      <c r="A65" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B65" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C65" s="10">
+      <c r="C65" s="11">
         <v>1.59126321E8</v>
       </c>
       <c r="D65" s="3">
         <v>2.0200328E7</v>
       </c>
-      <c r="E65" s="14">
+      <c r="E65" s="15">
         <v>10000.0</v>
       </c>
-      <c r="F65" s="14">
+      <c r="F65" s="15">
         <v>40000.0</v>
       </c>
-      <c r="G65" s="15" t="s">
-        <v>8</v>
+      <c r="G65" s="16" t="s">
+        <v>10</v>
       </c>
       <c r="H65" s="6">
         <v>0.0</v>
@@ -2138,25 +2148,25 @@
       <c r="I65" s="7"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="13" t="s">
-        <v>7</v>
+      <c r="A66" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C66" s="4">
         <v>5.8132461E8</v>
       </c>
-      <c r="D66" s="14">
+      <c r="D66" s="15">
         <v>2.0200328E7</v>
       </c>
-      <c r="E66" s="12">
-        <v>83000.0</v>
-      </c>
-      <c r="F66" s="12">
-        <v>123000.0</v>
-      </c>
-      <c r="G66" s="15" t="s">
+      <c r="E66" s="13">
+        <v>83000.0</v>
+      </c>
+      <c r="F66" s="13">
+        <v>123000.0</v>
+      </c>
+      <c r="G66" s="16" t="s">
         <v>2</v>
       </c>
       <c r="H66" s="6">
@@ -2165,26 +2175,26 @@
       <c r="I66" s="7"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B67" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C67" s="16">
+      <c r="A67" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C67" s="17">
         <v>4.68134129E8</v>
       </c>
-      <c r="D67" s="14">
+      <c r="D67" s="15">
         <v>2.0200329E7</v>
       </c>
-      <c r="E67" s="16">
-        <v>83000.0</v>
-      </c>
-      <c r="F67" s="16">
-        <v>123000.0</v>
-      </c>
-      <c r="G67" s="11" t="s">
-        <v>12</v>
+      <c r="E67" s="17">
+        <v>83000.0</v>
+      </c>
+      <c r="F67" s="17">
+        <v>123000.0</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>14</v>
       </c>
       <c r="H67" s="6">
         <v>0.0</v>
@@ -2192,25 +2202,25 @@
       <c r="I67" s="7"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B68" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C68" s="16">
+      <c r="A68" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C68" s="17">
         <v>1.23456871E8</v>
       </c>
-      <c r="D68" s="12">
+      <c r="D68" s="13">
         <v>2.0200327E7</v>
       </c>
-      <c r="E68" s="16">
-        <v>83000.0</v>
-      </c>
-      <c r="F68" s="16">
-        <v>123000.0</v>
-      </c>
-      <c r="G68" s="15" t="s">
+      <c r="E68" s="17">
+        <v>83000.0</v>
+      </c>
+      <c r="F68" s="17">
+        <v>123000.0</v>
+      </c>
+      <c r="G68" s="16" t="s">
         <v>2</v>
       </c>
       <c r="H68" s="6">
@@ -2219,11 +2229,11 @@
       <c r="I68" s="7"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="18" t="s">
-        <v>7</v>
+      <c r="A69" s="19" t="s">
+        <v>9</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C69" s="7">
         <v>1.23456871E8</v>
@@ -2231,14 +2241,14 @@
       <c r="D69" s="7">
         <v>2.0200327E7</v>
       </c>
-      <c r="E69" s="19">
+      <c r="E69" s="20">
         <v>10000.0</v>
       </c>
-      <c r="F69" s="19">
+      <c r="F69" s="20">
         <v>40000.0</v>
       </c>
-      <c r="G69" s="20" t="s">
-        <v>8</v>
+      <c r="G69" s="21" t="s">
+        <v>10</v>
       </c>
       <c r="H69" s="6">
         <v>0.0</v>
@@ -2246,11 +2256,11 @@
       <c r="I69" s="7"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B70" s="13" t="s">
-        <v>3</v>
+      <c r="A70" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>5</v>
       </c>
       <c r="C70" s="7">
         <v>1.23456871E8</v>
@@ -2264,7 +2274,7 @@
       <c r="F70" s="7">
         <v>162000.0</v>
       </c>
-      <c r="G70" s="20" t="s">
+      <c r="G70" s="21" t="s">
         <v>2</v>
       </c>
       <c r="H70" s="6">
@@ -2273,11 +2283,11 @@
       <c r="I70" s="7"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="18" t="s">
-        <v>7</v>
+      <c r="A71" s="19" t="s">
+        <v>9</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C71" s="4">
         <v>1.23456871E8</v>
@@ -2285,14 +2295,14 @@
       <c r="D71" s="4">
         <v>2.0200102E7</v>
       </c>
-      <c r="E71" s="12">
+      <c r="E71" s="13">
         <v>162200.0</v>
       </c>
-      <c r="F71" s="12">
+      <c r="F71" s="13">
         <v>162400.0</v>
       </c>
-      <c r="G71" s="20" t="s">
-        <v>8</v>
+      <c r="G71" s="21" t="s">
+        <v>10</v>
       </c>
       <c r="H71" s="6">
         <v>0.0</v>
@@ -2300,13 +2310,13 @@
       <c r="I71" s="7"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="18"/>
-      <c r="B72" s="21"/>
-      <c r="C72" s="21"/>
+      <c r="A72" s="19"/>
+      <c r="B72" s="22"/>
+      <c r="C72" s="22"/>
       <c r="D72" s="4"/>
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
-      <c r="G72" s="20"/>
+      <c r="G72" s="21"/>
       <c r="H72" s="4"/>
     </row>
     <row r="73" ht="15.75" customHeight="1"/>

</xml_diff>